<commit_message>
new jem form track
</commit_message>
<xml_diff>
--- a/Analysis/my_dataframe.xlsx
+++ b/Analysis/my_dataframe.xlsx
@@ -205,15 +205,15 @@
     <t>PAS4_171101_453_A01</t>
   </si>
   <si>
+    <t>PAS4_171102_451_A01</t>
+  </si>
+  <si>
+    <t>PAS4_171102_453_A01</t>
+  </si>
+  <si>
     <t>PAS4_171102_452_A01</t>
   </si>
   <si>
-    <t>PAS4_171102_453_A01</t>
-  </si>
-  <si>
-    <t>PAS4_171102_451_A01</t>
-  </si>
-  <si>
     <t>PAS4_171103_452_A01</t>
   </si>
   <si>
@@ -265,12 +265,12 @@
     <t>PAS4_171201_453_A01</t>
   </si>
   <si>
+    <t>PAS4_171201_451_A01</t>
+  </si>
+  <si>
     <t>PAS4_171201_452_A01</t>
   </si>
   <si>
-    <t>PAS4_171201_451_A01</t>
-  </si>
-  <si>
     <t>PAS4_171201_454_A01</t>
   </si>
   <si>
@@ -307,18 +307,18 @@
     <t>PAS4_171207_451_A01</t>
   </si>
   <si>
+    <t>PAS4_171207_454_A01</t>
+  </si>
+  <si>
+    <t>PAS4_171207_456_A01</t>
+  </si>
+  <si>
+    <t>PAS4_171207_455_A01</t>
+  </si>
+  <si>
     <t>PAS4_171207_453_A01</t>
   </si>
   <si>
-    <t>PAS4_171207_456_A01</t>
-  </si>
-  <si>
-    <t>PAS4_171207_455_A01</t>
-  </si>
-  <si>
-    <t>PAS4_171207_454_A01</t>
-  </si>
-  <si>
     <t>PAS4_171208_454_A01</t>
   </si>
   <si>
@@ -376,12 +376,12 @@
     <t>PAS4_180105_451_A01</t>
   </si>
   <si>
+    <t>PAS4_180108_451_A01</t>
+  </si>
+  <si>
     <t>PAS4_180108_452_A01</t>
   </si>
   <si>
-    <t>PAS4_180108_451_A01</t>
-  </si>
-  <si>
     <t>PAS4_180108_453_A01</t>
   </si>
   <si>
@@ -397,12 +397,12 @@
     <t>PAS4_180109_451_A01</t>
   </si>
   <si>
+    <t>PAS4_180110_451_A01</t>
+  </si>
+  <si>
     <t>PAS4_180110_452_A01</t>
   </si>
   <si>
-    <t>PAS4_180110_451_A01</t>
-  </si>
-  <si>
     <t>PAS4_180110_454_A01</t>
   </si>
   <si>
@@ -571,18 +571,18 @@
     <t>PAS4_180206_454_A01</t>
   </si>
   <si>
+    <t>PAS4_180207_454_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180207_455_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180207_451_A01</t>
+  </si>
+  <si>
     <t>PAS4_180207_453_A01</t>
   </si>
   <si>
-    <t>PAS4_180207_455_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180207_451_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180207_454_A01</t>
-  </si>
-  <si>
     <t>PAS4_180207_452_A01</t>
   </si>
   <si>
@@ -640,12 +640,12 @@
     <t>PAS4_180312_451_A01</t>
   </si>
   <si>
+    <t>PAS4_180313_453_A01</t>
+  </si>
+  <si>
     <t>PAS4_180313_451_A01</t>
   </si>
   <si>
-    <t>PAS4_180313_453_A01</t>
-  </si>
-  <si>
     <t>PAS4_180313_452_A01</t>
   </si>
   <si>
@@ -739,12 +739,12 @@
     <t>PAS4_180402_451_A01</t>
   </si>
   <si>
+    <t>PAS4_180403_452_A01</t>
+  </si>
+  <si>
     <t>PAS4_180403_451_A01</t>
   </si>
   <si>
-    <t>PAS4_180403_452_A01</t>
-  </si>
-  <si>
     <t>PAS4_180404_452_A01</t>
   </si>
   <si>
@@ -763,45 +763,45 @@
     <t>PAS4_180409_451_A01</t>
   </si>
   <si>
+    <t>PAS4_180411_452_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180411_453_A01</t>
+  </si>
+  <si>
     <t>PAS4_180411_451_A01</t>
   </si>
   <si>
-    <t>PAS4_180411_453_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180411_452_A01</t>
+    <t>PAS4_180413_452_A01</t>
   </si>
   <si>
     <t>PAS4_180413_451_A01</t>
   </si>
   <si>
-    <t>PAS4_180413_452_A01</t>
-  </si>
-  <si>
     <t>PAS4_180416_451_A01</t>
   </si>
   <si>
     <t>PAS4_180416_452_A01</t>
   </si>
   <si>
+    <t>PAS4_180417_455_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180417_453_A01</t>
+  </si>
+  <si>
     <t>PAS4_180417_454_A01</t>
   </si>
   <si>
-    <t>PAS4_180417_453_A01</t>
+    <t>PAS4_180417_451_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180417_452_A01</t>
   </si>
   <si>
     <t>PAS4_180417_456_A01</t>
   </si>
   <si>
-    <t>PAS4_180417_452_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180417_451_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180417_455_A01</t>
-  </si>
-  <si>
     <t>PAS4_180418_453_A01</t>
   </si>
   <si>
@@ -835,30 +835,30 @@
     <t>PAS4_180424_451_A01</t>
   </si>
   <si>
+    <t>PAS4_180424_458_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180424_456_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180424_455_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180424_457_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180424_454_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180424_452_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180424_453_A01</t>
+  </si>
+  <si>
     <t>PAS4_180424_459_A01</t>
   </si>
   <si>
-    <t>PAS4_180424_457_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180424_458_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180424_456_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180424_454_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180424_452_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180424_453_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180424_455_A01</t>
-  </si>
-  <si>
     <t>PAS4_180425_454_A01</t>
   </si>
   <si>
@@ -931,18 +931,18 @@
     <t>PAS4_180508_455_A01</t>
   </si>
   <si>
+    <t>PAS4_180508_452_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180508_453_A01</t>
+  </si>
+  <si>
     <t>PAS4_180508_451_A01</t>
   </si>
   <si>
     <t>PAS4_180508_454_A01</t>
   </si>
   <si>
-    <t>PAS4_180508_452_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180508_453_A01</t>
-  </si>
-  <si>
     <t>PAS4_180509_451_A01</t>
   </si>
   <si>
@@ -955,30 +955,30 @@
     <t>PAS4_180511_451_A01</t>
   </si>
   <si>
+    <t>PAS4_180514_451_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180514_453_A01</t>
+  </si>
+  <si>
     <t>PAS4_180514_452_A01</t>
   </si>
   <si>
-    <t>PAS4_180514_453_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180514_451_A01</t>
-  </si>
-  <si>
     <t>PAS4_180515_451_A01</t>
   </si>
   <si>
     <t>PAS4_180515_452_A01</t>
   </si>
   <si>
+    <t>PAS4_180516_454_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180516_451_A01</t>
+  </si>
+  <si>
     <t>PAS4_180516_455_A01</t>
   </si>
   <si>
-    <t>PAS4_180516_451_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180516_454_A01</t>
-  </si>
-  <si>
     <t>PAS4_180516_452_A01</t>
   </si>
   <si>
@@ -1000,18 +1000,18 @@
     <t>PAS4_180522_451_A01</t>
   </si>
   <si>
+    <t>PAS4_180523_451_A01</t>
+  </si>
+  <si>
     <t>PAS4_180523_452_A01</t>
   </si>
   <si>
-    <t>PAS4_180523_451_A01</t>
+    <t>PAS4_180524_451_A01</t>
   </si>
   <si>
     <t>PAS4_180524_452_A01</t>
   </si>
   <si>
-    <t>PAS4_180524_451_A01</t>
-  </si>
-  <si>
     <t>PAS4_180529_452_A01</t>
   </si>
   <si>
@@ -1093,12 +1093,12 @@
     <t>PAS4_180606_453_A01</t>
   </si>
   <si>
+    <t>PAS4_180606_452_A01</t>
+  </si>
+  <si>
     <t>PAS4_180606_451_A01</t>
   </si>
   <si>
-    <t>PAS4_180606_452_A01</t>
-  </si>
-  <si>
     <t>PAS4_180606_455_A01</t>
   </si>
   <si>
@@ -1114,15 +1114,15 @@
     <t>PAS4_180611_453_A01</t>
   </si>
   <si>
+    <t>PAS4_180612_454_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180612_453_A01</t>
+  </si>
+  <si>
     <t>PAS4_180612_455_A01</t>
   </si>
   <si>
-    <t>PAS4_180612_453_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180612_454_A01</t>
-  </si>
-  <si>
     <t>PAS4_180612_451_A01</t>
   </si>
   <si>
@@ -1132,18 +1132,18 @@
     <t>PAS4_180613_454_A01</t>
   </si>
   <si>
+    <t>PAS4_180613_451_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180613_453_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180613_455_A01</t>
+  </si>
+  <si>
     <t>PAS4_180613_452_A01</t>
   </si>
   <si>
-    <t>PAS4_180613_453_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180613_455_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180613_451_A01</t>
-  </si>
-  <si>
     <t>PAS4_180615_451_A01</t>
   </si>
   <si>
@@ -1204,15 +1204,15 @@
     <t>PAS4_180622_451_A01</t>
   </si>
   <si>
+    <t>PAS4_180622_453_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180622_454_A01</t>
+  </si>
+  <si>
     <t>PAS4_180622_452_A01</t>
   </si>
   <si>
-    <t>PAS4_180622_453_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180622_454_A01</t>
-  </si>
-  <si>
     <t>PAS4_180625_451_A01</t>
   </si>
   <si>
@@ -1225,12 +1225,12 @@
     <t>PAS4_180626_451_A01</t>
   </si>
   <si>
+    <t>PAS4_180627_454_A01</t>
+  </si>
+  <si>
     <t>PAS4_180627_455_A01</t>
   </si>
   <si>
-    <t>PAS4_180627_454_A01</t>
-  </si>
-  <si>
     <t>PAS4_180627_451_A01</t>
   </si>
   <si>
@@ -1291,12 +1291,12 @@
     <t>PAS4_180710_455_A01</t>
   </si>
   <si>
+    <t>PAS4_180710_452_A01</t>
+  </si>
+  <si>
     <t>PAS4_180710_451_A01</t>
   </si>
   <si>
-    <t>PAS4_180710_452_A01</t>
-  </si>
-  <si>
     <t>PAS4_180710_453_A01</t>
   </si>
   <si>
@@ -1306,18 +1306,18 @@
     <t>PAS4_180711_451_A01</t>
   </si>
   <si>
+    <t>PAS4_180711_455_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180711_454_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180711_453_A01</t>
+  </si>
+  <si>
     <t>PAS4_180711_452_A01</t>
   </si>
   <si>
-    <t>PAS4_180711_454_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180711_455_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180711_453_A01</t>
-  </si>
-  <si>
     <t>PAS4_180716_452_A01</t>
   </si>
   <si>
@@ -1351,12 +1351,12 @@
     <t>PAS4_180720_455_A01</t>
   </si>
   <si>
+    <t>PAS4_180720_452_A01</t>
+  </si>
+  <si>
     <t>PAS4_180720_451_A01</t>
   </si>
   <si>
-    <t>PAS4_180720_452_A01</t>
-  </si>
-  <si>
     <t>PAS4_180720_453_A01</t>
   </si>
   <si>
@@ -1456,36 +1456,36 @@
     <t>PAS4_180817_454_A01</t>
   </si>
   <si>
+    <t>PAS4_180817_453_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180817_452_A01</t>
+  </si>
+  <si>
     <t>PAS4_180817_455_A01</t>
   </si>
   <si>
-    <t>PAS4_180817_453_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180817_452_A01</t>
-  </si>
-  <si>
     <t>PAS4_180817_451_A01</t>
   </si>
   <si>
+    <t>PAS4_180820_452_A01</t>
+  </si>
+  <si>
     <t>PAS4_180820_451_A01</t>
   </si>
   <si>
-    <t>PAS4_180820_452_A01</t>
-  </si>
-  <si>
     <t>PAS4_180820_453_A01</t>
   </si>
   <si>
+    <t>PAS4_180820_455_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180820_454_A01</t>
+  </si>
+  <si>
     <t>PAS4_180820_456_A01</t>
   </si>
   <si>
-    <t>PAS4_180820_455_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180820_454_A01</t>
-  </si>
-  <si>
     <t>PAS4_180821_455_A01</t>
   </si>
   <si>
@@ -1528,36 +1528,36 @@
     <t>PAS4_180822_452_A01</t>
   </si>
   <si>
+    <t>PAS4_180823_455_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180823_451_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180823_454_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180823_456_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180823_452_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180823_453_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180823_458_A01</t>
+  </si>
+  <si>
     <t>PAS4_180823_457_A01</t>
   </si>
   <si>
-    <t>PAS4_180823_456_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180823_452_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180823_454_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180823_453_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180823_458_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180823_455_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180823_451_A01</t>
+    <t>PAS4_180823_461_A01</t>
   </si>
   <si>
     <t>PAS4_180823_460_A01</t>
   </si>
   <si>
-    <t>PAS4_180823_461_A01</t>
-  </si>
-  <si>
     <t>PAS4_180823_459_A01</t>
   </si>
   <si>
@@ -1573,27 +1573,27 @@
     <t>PAS4_180828_457_A01</t>
   </si>
   <si>
+    <t>PAS4_180828_458_A01</t>
+  </si>
+  <si>
     <t>PAS4_180828_459_A01</t>
   </si>
   <si>
-    <t>PAS4_180828_458_A01</t>
+    <t>PAS4_180828_456_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180828_452_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180828_454_A01</t>
   </si>
   <si>
     <t>PAS4_180828_455_A01</t>
   </si>
   <si>
-    <t>PAS4_180828_454_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180828_456_A01</t>
-  </si>
-  <si>
     <t>PAS4_180828_451_A01</t>
   </si>
   <si>
-    <t>PAS4_180828_452_A01</t>
-  </si>
-  <si>
     <t>PAS4_180828_453_A01</t>
   </si>
   <si>
@@ -1603,12 +1603,12 @@
     <t>PAS4_180829_451_A01</t>
   </si>
   <si>
+    <t>PAS4_180829_454_A01</t>
+  </si>
+  <si>
     <t>PAS4_180829_453_A01</t>
   </si>
   <si>
-    <t>PAS4_180829_454_A01</t>
-  </si>
-  <si>
     <t>PAS4_180829_455_A01</t>
   </si>
   <si>
@@ -1624,36 +1624,36 @@
     <t>PAS4_180830_453_A01</t>
   </si>
   <si>
+    <t>PAS4_180830_452_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180830_451_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180830_456_A01</t>
+  </si>
+  <si>
     <t>PAS4_180830_454_A01</t>
   </si>
   <si>
-    <t>PAS4_180830_451_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180830_456_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180830_452_A01</t>
+    <t>PAS4_180905_456_A01</t>
   </si>
   <si>
     <t>PAS4_180905_455_A01</t>
   </si>
   <si>
+    <t>PAS4_180905_451_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180905_453_A01</t>
+  </si>
+  <si>
     <t>PAS4_180905_454_A01</t>
   </si>
   <si>
-    <t>PAS4_180905_451_A01</t>
-  </si>
-  <si>
     <t>PAS4_180905_452_A01</t>
   </si>
   <si>
-    <t>PAS4_180905_456_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180905_453_A01</t>
-  </si>
-  <si>
     <t>PAS4_180906_451_A01</t>
   </si>
   <si>
@@ -1663,25 +1663,28 @@
     <t>PAS4_180906_456_A01</t>
   </si>
   <si>
+    <t>PAS4_180906_453_A01</t>
+  </si>
+  <si>
+    <t>PAS4_180906_452_A01</t>
+  </si>
+  <si>
     <t>PAS4_180906_454_A01</t>
   </si>
   <si>
-    <t>PAS4_180906_453_A01</t>
-  </si>
-  <si>
-    <t>PAS4_180906_452_A01</t>
-  </si>
-  <si>
     <t>PAS4_180906_457_A01</t>
   </si>
   <si>
     <t>PAS4_180907_452_A01</t>
   </si>
   <si>
+    <t>PAS4_180907_454_A01</t>
+  </si>
+  <si>
     <t>PAS4_180907_453_A01</t>
   </si>
   <si>
-    <t>PAS4_180907_454_A01</t>
+    <t>PAS4_180907_457_A01</t>
   </si>
   <si>
     <t>PAS4_180907_456_A01</t>
@@ -1690,9 +1693,6 @@
     <t>PAS4_180907_455_A01</t>
   </si>
   <si>
-    <t>PAS4_180907_457_A01</t>
-  </si>
-  <si>
     <t>PAS4_180907_451_A01</t>
   </si>
   <si>
@@ -1912,22 +1912,22 @@
     <t>Sst Chrna2 Ptgdr</t>
   </si>
   <si>
+    <t>n74</t>
+  </si>
+  <si>
     <t>n108</t>
   </si>
   <si>
-    <t>n74</t>
-  </si>
-  <si>
     <t>n114</t>
   </si>
   <si>
     <t>n100</t>
   </si>
   <si>
+    <t>Inh L1-4 LAMP5 LCP2 (rosehip)</t>
+  </si>
+  <si>
     <t>Excitatory</t>
-  </si>
-  <si>
-    <t>Inh L1-4 LAMP5 LCP2 (rosehip)</t>
   </si>
   <si>
     <t>Sst Chrna2 Glra3</t>
@@ -4340,13 +4340,13 @@
         <v>563</v>
       </c>
       <c r="F55">
-        <v>28.09999999999991</v>
+        <v>36.19999999999982</v>
       </c>
       <c r="G55">
-        <v>-32</v>
+        <v>-37</v>
       </c>
       <c r="H55">
-        <v>10.38333333333333</v>
+        <v>9.25</v>
       </c>
       <c r="I55" t="s">
         <v>572</v>
@@ -4410,13 +4410,13 @@
         <v>563</v>
       </c>
       <c r="F57">
-        <v>36.19999999999982</v>
+        <v>28.09999999999991</v>
       </c>
       <c r="G57">
-        <v>-37</v>
+        <v>-32</v>
       </c>
       <c r="H57">
-        <v>9.25</v>
+        <v>10.38333333333333</v>
       </c>
       <c r="I57" t="s">
         <v>572</v>
@@ -5037,25 +5037,25 @@
         <v>560</v>
       </c>
       <c r="E75" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F75">
-        <v>38</v>
+        <v>57.5</v>
       </c>
       <c r="G75">
-        <v>-37</v>
+        <v>70</v>
       </c>
       <c r="H75">
-        <v>10.41666666666667</v>
+        <v>5.483333333333333</v>
       </c>
       <c r="I75" t="s">
         <v>571</v>
       </c>
       <c r="J75">
-        <v>0.604422452</v>
+        <v>0.883982313</v>
       </c>
       <c r="K75" t="s">
-        <v>594</v>
+        <v>611</v>
       </c>
     </row>
     <row r="76" spans="1:11">
@@ -5072,25 +5072,25 @@
         <v>560</v>
       </c>
       <c r="E76" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F76">
-        <v>57.5</v>
+        <v>38</v>
       </c>
       <c r="G76">
-        <v>70</v>
+        <v>-37</v>
       </c>
       <c r="H76">
-        <v>5.483333333333333</v>
+        <v>10.41666666666667</v>
       </c>
       <c r="I76" t="s">
         <v>571</v>
       </c>
       <c r="J76">
-        <v>0.883982313</v>
+        <v>0.604422452</v>
       </c>
       <c r="K76" t="s">
-        <v>611</v>
+        <v>594</v>
       </c>
     </row>
     <row r="77" spans="1:11">
@@ -5527,16 +5527,16 @@
         <v>560</v>
       </c>
       <c r="E89" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F89">
-        <v>30.19999999999981</v>
+        <v>28.90000000000055</v>
       </c>
       <c r="G89">
         <v>-40</v>
       </c>
       <c r="H89">
-        <v>8.75</v>
+        <v>8.566666666666666</v>
       </c>
       <c r="I89" t="s">
         <v>572</v>
@@ -5545,7 +5545,7 @@
         <v>1</v>
       </c>
       <c r="K89" t="s">
-        <v>615</v>
+        <v>589</v>
       </c>
     </row>
     <row r="90" spans="1:11">
@@ -5632,16 +5632,16 @@
         <v>560</v>
       </c>
       <c r="E92" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F92">
-        <v>28.90000000000055</v>
+        <v>30.19999999999981</v>
       </c>
       <c r="G92">
         <v>-40</v>
       </c>
       <c r="H92">
-        <v>8.566666666666666</v>
+        <v>8.75</v>
       </c>
       <c r="I92" t="s">
         <v>572</v>
@@ -5650,7 +5650,7 @@
         <v>1</v>
       </c>
       <c r="K92" t="s">
-        <v>589</v>
+        <v>615</v>
       </c>
     </row>
     <row r="93" spans="1:11">
@@ -6332,25 +6332,25 @@
         <v>560</v>
       </c>
       <c r="E112" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F112">
-        <v>52</v>
+        <v>45.4</v>
       </c>
       <c r="G112">
         <v>-40</v>
       </c>
       <c r="H112">
-        <v>10.85</v>
+        <v>11.16666666666667</v>
       </c>
       <c r="I112" t="s">
         <v>572</v>
       </c>
       <c r="J112">
-        <v>1</v>
+        <v>0.467256505</v>
       </c>
       <c r="K112" t="s">
-        <v>578</v>
+        <v>621</v>
       </c>
     </row>
     <row r="113" spans="1:11">
@@ -6367,25 +6367,25 @@
         <v>560</v>
       </c>
       <c r="E113" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="F113">
-        <v>45.4</v>
+        <v>52</v>
       </c>
       <c r="G113">
         <v>-40</v>
       </c>
       <c r="H113">
-        <v>11.16666666666667</v>
+        <v>10.85</v>
       </c>
       <c r="I113" t="s">
         <v>572</v>
       </c>
       <c r="J113">
-        <v>0.467256505</v>
+        <v>1</v>
       </c>
       <c r="K113" t="s">
-        <v>621</v>
+        <v>578</v>
       </c>
     </row>
     <row r="114" spans="1:11">
@@ -6580,22 +6580,22 @@
         <v>564</v>
       </c>
       <c r="F119">
-        <v>17.8</v>
+        <v>63.7</v>
       </c>
       <c r="G119">
-        <v>-25</v>
+        <v>-35</v>
       </c>
       <c r="H119">
-        <v>9.683333333333334</v>
+        <v>10.75</v>
       </c>
       <c r="I119" t="s">
         <v>572</v>
       </c>
       <c r="J119">
-        <v>0.714428417</v>
+        <v>1</v>
       </c>
       <c r="K119" t="s">
-        <v>581</v>
+        <v>592</v>
       </c>
     </row>
     <row r="120" spans="1:11">
@@ -6615,22 +6615,22 @@
         <v>564</v>
       </c>
       <c r="F120">
-        <v>63.7</v>
+        <v>17.8</v>
       </c>
       <c r="G120">
-        <v>-35</v>
+        <v>-25</v>
       </c>
       <c r="H120">
-        <v>10.75</v>
+        <v>9.683333333333334</v>
       </c>
       <c r="I120" t="s">
         <v>572</v>
       </c>
       <c r="J120">
-        <v>1</v>
+        <v>0.714428417</v>
       </c>
       <c r="K120" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
     </row>
     <row r="121" spans="1:11">
@@ -8610,22 +8610,22 @@
         <v>565</v>
       </c>
       <c r="F177">
-        <v>32.90000000000145</v>
+        <v>35.30000000000109</v>
       </c>
       <c r="G177">
-        <v>-20</v>
+        <v>-18</v>
       </c>
       <c r="H177">
-        <v>9.35</v>
+        <v>9.966666666666667</v>
       </c>
       <c r="I177" t="s">
         <v>572</v>
       </c>
       <c r="J177">
-        <v>0.542000997</v>
+        <v>0.898196715</v>
       </c>
       <c r="K177" t="s">
-        <v>610</v>
+        <v>632</v>
       </c>
     </row>
     <row r="178" spans="1:11">
@@ -8695,7 +8695,7 @@
         <v>0.8440999890000001</v>
       </c>
       <c r="K179" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="180" spans="1:11">
@@ -8715,22 +8715,22 @@
         <v>565</v>
       </c>
       <c r="F180">
-        <v>35.30000000000109</v>
+        <v>32.90000000000145</v>
       </c>
       <c r="G180">
-        <v>-18</v>
+        <v>-20</v>
       </c>
       <c r="H180">
-        <v>9.966666666666667</v>
+        <v>9.35</v>
       </c>
       <c r="I180" t="s">
         <v>572</v>
       </c>
       <c r="J180">
-        <v>0.898196715</v>
+        <v>0.542000997</v>
       </c>
       <c r="K180" t="s">
-        <v>633</v>
+        <v>610</v>
       </c>
     </row>
     <row r="181" spans="1:11">
@@ -9412,22 +9412,22 @@
         <v>561</v>
       </c>
       <c r="E200" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="F200">
-        <v>30.89999999999998</v>
+        <v>33.10000000000002</v>
       </c>
       <c r="G200">
-        <v>-31</v>
+        <v>-26</v>
       </c>
       <c r="H200">
-        <v>21.98333333333333</v>
+        <v>23.68333333333333</v>
       </c>
       <c r="I200" t="s">
         <v>572</v>
       </c>
       <c r="J200">
-        <v>0.365140676</v>
+        <v>1</v>
       </c>
       <c r="K200" t="s">
         <v>636</v>
@@ -9447,22 +9447,22 @@
         <v>561</v>
       </c>
       <c r="E201" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="F201">
-        <v>33.10000000000002</v>
+        <v>30.89999999999998</v>
       </c>
       <c r="G201">
-        <v>-26</v>
+        <v>-31</v>
       </c>
       <c r="H201">
-        <v>23.68333333333333</v>
+        <v>21.98333333333333</v>
       </c>
       <c r="I201" t="s">
         <v>572</v>
       </c>
       <c r="J201">
-        <v>1</v>
+        <v>0.365140676</v>
       </c>
       <c r="K201" t="s">
         <v>637</v>
@@ -9500,7 +9500,7 @@
         <v>0.365140676</v>
       </c>
       <c r="K202" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="203" spans="1:11">
@@ -10570,22 +10570,22 @@
         <v>564</v>
       </c>
       <c r="F233">
-        <v>44.30000000000018</v>
+        <v>56.80000000000018</v>
       </c>
       <c r="G233">
-        <v>-26</v>
+        <v>-42</v>
       </c>
       <c r="H233">
-        <v>6.8</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="I233" t="s">
         <v>571</v>
       </c>
       <c r="J233">
-        <v>0.714428417</v>
+        <v>0.467256505</v>
       </c>
       <c r="K233" t="s">
-        <v>581</v>
+        <v>621</v>
       </c>
     </row>
     <row r="234" spans="1:11">
@@ -10605,22 +10605,22 @@
         <v>564</v>
       </c>
       <c r="F234">
-        <v>56.80000000000018</v>
+        <v>44.30000000000018</v>
       </c>
       <c r="G234">
-        <v>-42</v>
+        <v>-26</v>
       </c>
       <c r="H234">
-        <v>8.699999999999999</v>
+        <v>6.8</v>
       </c>
       <c r="I234" t="s">
         <v>571</v>
       </c>
       <c r="J234">
-        <v>0.467256505</v>
+        <v>0.714428417</v>
       </c>
       <c r="K234" t="s">
-        <v>621</v>
+        <v>581</v>
       </c>
     </row>
     <row r="235" spans="1:11">
@@ -10847,16 +10847,16 @@
         <v>560</v>
       </c>
       <c r="E241" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F241">
-        <v>40.30000000000018</v>
+        <v>26.40000000000009</v>
       </c>
       <c r="G241">
         <v>-35</v>
       </c>
       <c r="H241">
-        <v>8.783333333333333</v>
+        <v>12.58333333333333</v>
       </c>
       <c r="I241" t="s">
         <v>572</v>
@@ -10865,7 +10865,7 @@
         <v>1</v>
       </c>
       <c r="K241" t="s">
-        <v>582</v>
+        <v>616</v>
       </c>
     </row>
     <row r="242" spans="1:11">
@@ -10917,16 +10917,16 @@
         <v>560</v>
       </c>
       <c r="E243" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="F243">
-        <v>26.40000000000009</v>
+        <v>40.30000000000018</v>
       </c>
       <c r="G243">
         <v>-35</v>
       </c>
       <c r="H243">
-        <v>12.58333333333333</v>
+        <v>8.783333333333333</v>
       </c>
       <c r="I243" t="s">
         <v>572</v>
@@ -10935,7 +10935,7 @@
         <v>1</v>
       </c>
       <c r="K243" t="s">
-        <v>616</v>
+        <v>582</v>
       </c>
     </row>
     <row r="244" spans="1:11">
@@ -10955,13 +10955,13 @@
         <v>563</v>
       </c>
       <c r="F244">
-        <v>52.5999999999999</v>
+        <v>40.70000000000027</v>
       </c>
       <c r="G244">
         <v>-40</v>
       </c>
       <c r="H244">
-        <v>10.1</v>
+        <v>9.949999999999999</v>
       </c>
       <c r="I244" t="s">
         <v>572</v>
@@ -10970,7 +10970,7 @@
         <v>1</v>
       </c>
       <c r="K244" t="s">
-        <v>603</v>
+        <v>620</v>
       </c>
     </row>
     <row r="245" spans="1:11">
@@ -10990,13 +10990,13 @@
         <v>563</v>
       </c>
       <c r="F245">
-        <v>40.70000000000027</v>
+        <v>52.5999999999999</v>
       </c>
       <c r="G245">
         <v>-40</v>
       </c>
       <c r="H245">
-        <v>9.949999999999999</v>
+        <v>10.1</v>
       </c>
       <c r="I245" t="s">
         <v>572</v>
@@ -11005,7 +11005,7 @@
         <v>1</v>
       </c>
       <c r="K245" t="s">
-        <v>620</v>
+        <v>603</v>
       </c>
     </row>
     <row r="246" spans="1:11">
@@ -11095,22 +11095,22 @@
         <v>567</v>
       </c>
       <c r="F248">
-        <v>96.8000000000002</v>
+        <v>61.80000000000018</v>
       </c>
       <c r="G248">
-        <v>-40</v>
+        <v>-44</v>
       </c>
       <c r="H248">
-        <v>22.61666666666667</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="I248" t="s">
         <v>571</v>
       </c>
       <c r="J248">
-        <v>0.365140676</v>
+        <v>0</v>
       </c>
       <c r="K248" t="s">
-        <v>636</v>
+        <v>612</v>
       </c>
     </row>
     <row r="249" spans="1:11">
@@ -11165,22 +11165,22 @@
         <v>567</v>
       </c>
       <c r="F250">
-        <v>39.20000000000027</v>
+        <v>96.8000000000002</v>
       </c>
       <c r="G250">
-        <v>-41</v>
+        <v>-40</v>
       </c>
       <c r="H250">
-        <v>23.86666666666667</v>
+        <v>22.61666666666667</v>
       </c>
       <c r="I250" t="s">
         <v>571</v>
       </c>
       <c r="J250">
-        <v>0</v>
+        <v>0.365140676</v>
       </c>
       <c r="K250" t="s">
-        <v>612</v>
+        <v>637</v>
       </c>
     </row>
     <row r="251" spans="1:11">
@@ -11197,25 +11197,25 @@
         <v>560</v>
       </c>
       <c r="E251" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F251">
-        <v>53.5999999999999</v>
+        <v>36.69999999999982</v>
       </c>
       <c r="G251">
-        <v>-25</v>
+        <v>-36</v>
       </c>
       <c r="H251">
-        <v>10.15</v>
+        <v>9.283333333333333</v>
       </c>
       <c r="I251" t="s">
         <v>573</v>
       </c>
       <c r="J251">
-        <v>0.714428417</v>
+        <v>0.291080192</v>
       </c>
       <c r="K251" t="s">
-        <v>581</v>
+        <v>590</v>
       </c>
     </row>
     <row r="252" spans="1:11">
@@ -11232,25 +11232,25 @@
         <v>560</v>
       </c>
       <c r="E252" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="F252">
-        <v>36.69999999999982</v>
+        <v>53.5999999999999</v>
       </c>
       <c r="G252">
-        <v>-36</v>
+        <v>-25</v>
       </c>
       <c r="H252">
-        <v>9.283333333333333</v>
+        <v>10.15</v>
       </c>
       <c r="I252" t="s">
         <v>573</v>
       </c>
       <c r="J252">
-        <v>0.291080192</v>
+        <v>0.714428417</v>
       </c>
       <c r="K252" t="s">
-        <v>590</v>
+        <v>581</v>
       </c>
     </row>
     <row r="253" spans="1:11">
@@ -11270,13 +11270,13 @@
         <v>567</v>
       </c>
       <c r="F253">
-        <v>61.80000000000018</v>
+        <v>39.20000000000027</v>
       </c>
       <c r="G253">
-        <v>-44</v>
+        <v>-41</v>
       </c>
       <c r="H253">
-        <v>9.800000000000001</v>
+        <v>23.86666666666667</v>
       </c>
       <c r="I253" t="s">
         <v>571</v>
@@ -11687,16 +11687,16 @@
         <v>562</v>
       </c>
       <c r="E265" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="F265">
-        <v>63</v>
+        <v>62.30000000000018</v>
       </c>
       <c r="G265">
-        <v>-26</v>
+        <v>-38</v>
       </c>
       <c r="H265">
-        <v>13.86666666666667</v>
+        <v>20.9</v>
       </c>
       <c r="I265" t="s">
         <v>571</v>
@@ -11725,13 +11725,13 @@
         <v>567</v>
       </c>
       <c r="F266">
-        <v>44.5</v>
+        <v>61.9000000000001</v>
       </c>
       <c r="G266">
-        <v>-40</v>
+        <v>-54</v>
       </c>
       <c r="H266">
-        <v>7.433333333333334</v>
+        <v>24.81666666666667</v>
       </c>
       <c r="I266" t="s">
         <v>573</v>
@@ -11757,16 +11757,16 @@
         <v>562</v>
       </c>
       <c r="E267" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="F267">
-        <v>62.30000000000018</v>
+        <v>69.09999999999991</v>
       </c>
       <c r="G267">
-        <v>-38</v>
+        <v>-40</v>
       </c>
       <c r="H267">
-        <v>20.9</v>
+        <v>21</v>
       </c>
       <c r="I267" t="s">
         <v>571</v>
@@ -11795,13 +11795,13 @@
         <v>567</v>
       </c>
       <c r="F268">
-        <v>61.9000000000001</v>
+        <v>44.5</v>
       </c>
       <c r="G268">
-        <v>-54</v>
+        <v>-40</v>
       </c>
       <c r="H268">
-        <v>24.81666666666667</v>
+        <v>7.433333333333334</v>
       </c>
       <c r="I268" t="s">
         <v>573</v>
@@ -11932,16 +11932,16 @@
         <v>562</v>
       </c>
       <c r="E272" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="F272">
-        <v>69.09999999999991</v>
+        <v>63</v>
       </c>
       <c r="G272">
-        <v>-40</v>
+        <v>-26</v>
       </c>
       <c r="H272">
-        <v>21</v>
+        <v>13.86666666666667</v>
       </c>
       <c r="I272" t="s">
         <v>571</v>
@@ -12810,22 +12810,22 @@
         <v>565</v>
       </c>
       <c r="F297">
-        <v>43.5</v>
+        <v>48.10000000000002</v>
       </c>
       <c r="G297">
-        <v>-28</v>
+        <v>-30</v>
       </c>
       <c r="H297">
-        <v>8.866666666666667</v>
+        <v>16.08333333333333</v>
       </c>
       <c r="I297" t="s">
         <v>572</v>
       </c>
       <c r="J297">
-        <v>0.5482247220000001</v>
+        <v>1</v>
       </c>
       <c r="K297" t="s">
-        <v>577</v>
+        <v>605</v>
       </c>
     </row>
     <row r="298" spans="1:11">
@@ -12845,22 +12845,22 @@
         <v>564</v>
       </c>
       <c r="F298">
-        <v>40.70000000000005</v>
+        <v>40.29999999999996</v>
       </c>
       <c r="G298">
-        <v>-30</v>
+        <v>-33</v>
       </c>
       <c r="H298">
-        <v>8.133333333333333</v>
+        <v>10.3</v>
       </c>
       <c r="I298" t="s">
         <v>572</v>
       </c>
       <c r="J298">
-        <v>0.291080192</v>
+        <v>0.7916152479999999</v>
       </c>
       <c r="K298" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
     </row>
     <row r="299" spans="1:11">
@@ -12880,22 +12880,22 @@
         <v>565</v>
       </c>
       <c r="F299">
-        <v>48.10000000000002</v>
+        <v>43.5</v>
       </c>
       <c r="G299">
-        <v>-30</v>
+        <v>-28</v>
       </c>
       <c r="H299">
-        <v>16.08333333333333</v>
+        <v>8.866666666666667</v>
       </c>
       <c r="I299" t="s">
         <v>572</v>
       </c>
       <c r="J299">
-        <v>1</v>
+        <v>0.5482247220000001</v>
       </c>
       <c r="K299" t="s">
-        <v>605</v>
+        <v>577</v>
       </c>
     </row>
     <row r="300" spans="1:11">
@@ -12915,22 +12915,22 @@
         <v>564</v>
       </c>
       <c r="F300">
-        <v>40.29999999999996</v>
+        <v>40.70000000000005</v>
       </c>
       <c r="G300">
-        <v>-33</v>
+        <v>-30</v>
       </c>
       <c r="H300">
-        <v>10.3</v>
+        <v>8.133333333333333</v>
       </c>
       <c r="I300" t="s">
         <v>572</v>
       </c>
       <c r="J300">
-        <v>0.7916152479999999</v>
+        <v>0.291080192</v>
       </c>
       <c r="K300" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="301" spans="1:11">
@@ -13087,25 +13087,25 @@
         <v>560</v>
       </c>
       <c r="E305" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="F305">
-        <v>36</v>
+        <v>39.70000000000005</v>
       </c>
       <c r="G305">
-        <v>-26</v>
+        <v>-25</v>
       </c>
       <c r="H305">
-        <v>10.66666666666667</v>
+        <v>11.18333333333333</v>
       </c>
       <c r="I305" t="s">
         <v>572</v>
       </c>
       <c r="J305">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K305" t="s">
-        <v>655</v>
+        <v>583</v>
       </c>
     </row>
     <row r="306" spans="1:11">
@@ -13157,25 +13157,25 @@
         <v>560</v>
       </c>
       <c r="E307" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F307">
-        <v>39.70000000000005</v>
+        <v>36</v>
       </c>
       <c r="G307">
-        <v>-25</v>
+        <v>-26</v>
       </c>
       <c r="H307">
-        <v>11.18333333333333</v>
+        <v>10.66666666666667</v>
       </c>
       <c r="I307" t="s">
         <v>572</v>
       </c>
       <c r="J307">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K307" t="s">
-        <v>583</v>
+        <v>655</v>
       </c>
     </row>
     <row r="308" spans="1:11">
@@ -13265,22 +13265,22 @@
         <v>564</v>
       </c>
       <c r="F310">
-        <v>31.20000000000005</v>
+        <v>57.69999999999993</v>
       </c>
       <c r="G310">
-        <v>-35</v>
+        <v>-25</v>
       </c>
       <c r="H310">
-        <v>7.75</v>
+        <v>9.133333333333333</v>
       </c>
       <c r="I310" t="s">
         <v>571</v>
       </c>
       <c r="J310">
-        <v>0.83662843</v>
+        <v>0.542000997</v>
       </c>
       <c r="K310" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
     </row>
     <row r="311" spans="1:11">
@@ -13335,22 +13335,22 @@
         <v>564</v>
       </c>
       <c r="F312">
-        <v>57.69999999999993</v>
+        <v>31.20000000000005</v>
       </c>
       <c r="G312">
-        <v>-25</v>
+        <v>-35</v>
       </c>
       <c r="H312">
-        <v>9.133333333333333</v>
+        <v>7.75</v>
       </c>
       <c r="I312" t="s">
         <v>571</v>
       </c>
       <c r="J312">
-        <v>0.542000997</v>
+        <v>0.83662843</v>
       </c>
       <c r="K312" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="313" spans="1:11">
@@ -13595,7 +13595,7 @@
         <v>0.365140676</v>
       </c>
       <c r="K319" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="320" spans="1:11">
@@ -13612,25 +13612,25 @@
         <v>560</v>
       </c>
       <c r="E320" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="F320">
-        <v>47</v>
+        <v>31.30000000000007</v>
       </c>
       <c r="G320">
-        <v>-30</v>
+        <v>-33</v>
       </c>
       <c r="H320">
-        <v>9.9</v>
+        <v>8.550000000000001</v>
       </c>
       <c r="I320" t="s">
         <v>572</v>
       </c>
       <c r="J320">
-        <v>0.434668865</v>
+        <v>1</v>
       </c>
       <c r="K320" t="s">
-        <v>576</v>
+        <v>582</v>
       </c>
     </row>
     <row r="321" spans="1:11">
@@ -13647,25 +13647,25 @@
         <v>560</v>
       </c>
       <c r="E321" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F321">
-        <v>31.30000000000007</v>
+        <v>47</v>
       </c>
       <c r="G321">
-        <v>-33</v>
+        <v>-30</v>
       </c>
       <c r="H321">
-        <v>8.550000000000001</v>
+        <v>9.9</v>
       </c>
       <c r="I321" t="s">
         <v>572</v>
       </c>
       <c r="J321">
-        <v>1</v>
+        <v>0.434668865</v>
       </c>
       <c r="K321" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
     </row>
     <row r="322" spans="1:11">
@@ -13682,25 +13682,25 @@
         <v>560</v>
       </c>
       <c r="E322" t="s">
-        <v>563</v>
+        <v>568</v>
       </c>
       <c r="F322">
-        <v>35.39999999999998</v>
+        <v>30.10000000000002</v>
       </c>
       <c r="G322">
-        <v>-26</v>
+        <v>-40</v>
       </c>
       <c r="H322">
-        <v>15.01666666666667</v>
+        <v>7.716666666666667</v>
       </c>
       <c r="I322" t="s">
         <v>572</v>
       </c>
       <c r="J322">
-        <v>1</v>
+        <v>0.860418943</v>
       </c>
       <c r="K322" t="s">
-        <v>656</v>
+        <v>635</v>
       </c>
     </row>
     <row r="323" spans="1:11">
@@ -13717,25 +13717,25 @@
         <v>560</v>
       </c>
       <c r="E323" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="F323">
-        <v>30.10000000000002</v>
+        <v>35.39999999999998</v>
       </c>
       <c r="G323">
-        <v>-40</v>
+        <v>-26</v>
       </c>
       <c r="H323">
-        <v>7.716666666666667</v>
+        <v>15.01666666666667</v>
       </c>
       <c r="I323" t="s">
         <v>572</v>
       </c>
       <c r="J323">
-        <v>0.860418943</v>
+        <v>1</v>
       </c>
       <c r="K323" t="s">
-        <v>635</v>
+        <v>656</v>
       </c>
     </row>
     <row r="324" spans="1:11">
@@ -14697,25 +14697,25 @@
         <v>560</v>
       </c>
       <c r="E351" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F351">
-        <v>43.80000000000001</v>
+        <v>53</v>
       </c>
       <c r="G351">
         <v>-25</v>
       </c>
       <c r="H351">
-        <v>16.43333333333333</v>
+        <v>13.6</v>
       </c>
       <c r="I351" t="s">
         <v>571</v>
       </c>
       <c r="J351">
-        <v>0.5809745079999999</v>
+        <v>0.291080192</v>
       </c>
       <c r="K351" t="s">
-        <v>666</v>
+        <v>590</v>
       </c>
     </row>
     <row r="352" spans="1:11">
@@ -14732,25 +14732,25 @@
         <v>560</v>
       </c>
       <c r="E352" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="F352">
-        <v>53</v>
+        <v>43.80000000000001</v>
       </c>
       <c r="G352">
         <v>-25</v>
       </c>
       <c r="H352">
-        <v>13.6</v>
+        <v>16.43333333333333</v>
       </c>
       <c r="I352" t="s">
         <v>571</v>
       </c>
       <c r="J352">
-        <v>0.291080192</v>
+        <v>0.5809745079999999</v>
       </c>
       <c r="K352" t="s">
-        <v>590</v>
+        <v>666</v>
       </c>
     </row>
     <row r="353" spans="1:11">
@@ -14942,16 +14942,16 @@
         <v>560</v>
       </c>
       <c r="E358" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="F358">
-        <v>43.5</v>
+        <v>40.6</v>
       </c>
       <c r="G358">
-        <v>-30</v>
+        <v>-25</v>
       </c>
       <c r="H358">
-        <v>15.85</v>
+        <v>14.88333333333333</v>
       </c>
       <c r="I358" t="s">
         <v>572</v>
@@ -14960,7 +14960,7 @@
         <v>1</v>
       </c>
       <c r="K358" t="s">
-        <v>603</v>
+        <v>615</v>
       </c>
     </row>
     <row r="359" spans="1:11">
@@ -15012,16 +15012,16 @@
         <v>560</v>
       </c>
       <c r="E360" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="F360">
-        <v>40.6</v>
+        <v>43.5</v>
       </c>
       <c r="G360">
-        <v>-25</v>
+        <v>-30</v>
       </c>
       <c r="H360">
-        <v>14.88333333333333</v>
+        <v>15.85</v>
       </c>
       <c r="I360" t="s">
         <v>572</v>
@@ -15030,7 +15030,7 @@
         <v>1</v>
       </c>
       <c r="K360" t="s">
-        <v>615</v>
+        <v>603</v>
       </c>
     </row>
     <row r="361" spans="1:11">
@@ -15155,22 +15155,22 @@
         <v>564</v>
       </c>
       <c r="F364">
-        <v>37.4</v>
+        <v>29.90000000000001</v>
       </c>
       <c r="G364">
-        <v>-20</v>
+        <v>-25</v>
       </c>
       <c r="H364">
-        <v>9.15</v>
+        <v>15.05</v>
       </c>
       <c r="I364" t="s">
         <v>575</v>
       </c>
       <c r="J364">
-        <v>1</v>
+        <v>0.6724663670000001</v>
       </c>
       <c r="K364" t="s">
-        <v>655</v>
+        <v>624</v>
       </c>
     </row>
     <row r="365" spans="1:11">
@@ -15260,22 +15260,22 @@
         <v>564</v>
       </c>
       <c r="F367">
-        <v>29.90000000000001</v>
+        <v>37.4</v>
       </c>
       <c r="G367">
-        <v>-25</v>
+        <v>-20</v>
       </c>
       <c r="H367">
-        <v>15.05</v>
+        <v>9.15</v>
       </c>
       <c r="I367" t="s">
         <v>575</v>
       </c>
       <c r="J367">
-        <v>0.6724663670000001</v>
+        <v>1</v>
       </c>
       <c r="K367" t="s">
-        <v>624</v>
+        <v>655</v>
       </c>
     </row>
     <row r="368" spans="1:11">
@@ -15415,7 +15415,7 @@
         <v>0.898196715</v>
       </c>
       <c r="K371" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="372" spans="1:11">
@@ -15995,22 +15995,22 @@
         <v>565</v>
       </c>
       <c r="F388">
-        <v>38.3</v>
+        <v>42.7</v>
       </c>
       <c r="G388">
-        <v>-40</v>
+        <v>-24</v>
       </c>
       <c r="H388">
-        <v>9.266666666666667</v>
+        <v>8.333333333333334</v>
       </c>
       <c r="I388" t="s">
         <v>572</v>
       </c>
       <c r="J388">
-        <v>0.714428417</v>
+        <v>1</v>
       </c>
       <c r="K388" t="s">
-        <v>581</v>
+        <v>627</v>
       </c>
     </row>
     <row r="389" spans="1:11">
@@ -16027,16 +16027,16 @@
         <v>560</v>
       </c>
       <c r="E389" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F389">
-        <v>42.7</v>
+        <v>37.99999999999999</v>
       </c>
       <c r="G389">
-        <v>-24</v>
+        <v>-35</v>
       </c>
       <c r="H389">
-        <v>8.333333333333334</v>
+        <v>8.933333333333334</v>
       </c>
       <c r="I389" t="s">
         <v>572</v>
@@ -16045,7 +16045,7 @@
         <v>1</v>
       </c>
       <c r="K389" t="s">
-        <v>627</v>
+        <v>616</v>
       </c>
     </row>
     <row r="390" spans="1:11">
@@ -16062,25 +16062,25 @@
         <v>560</v>
       </c>
       <c r="E390" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="F390">
-        <v>37.99999999999999</v>
+        <v>38.3</v>
       </c>
       <c r="G390">
-        <v>-35</v>
+        <v>-40</v>
       </c>
       <c r="H390">
-        <v>8.933333333333334</v>
+        <v>9.266666666666667</v>
       </c>
       <c r="I390" t="s">
         <v>572</v>
       </c>
       <c r="J390">
-        <v>1</v>
+        <v>0.714428417</v>
       </c>
       <c r="K390" t="s">
-        <v>616</v>
+        <v>581</v>
       </c>
     </row>
     <row r="391" spans="1:11">
@@ -16240,22 +16240,22 @@
         <v>565</v>
       </c>
       <c r="F395">
-        <v>51.30000000000001</v>
+        <v>55.10000000000001</v>
       </c>
       <c r="G395">
         <v>-25</v>
       </c>
       <c r="H395">
-        <v>10.86666666666667</v>
+        <v>8.866666666666667</v>
       </c>
       <c r="I395" t="s">
         <v>572</v>
       </c>
       <c r="J395">
-        <v>0.700977107</v>
+        <v>0.604422452</v>
       </c>
       <c r="K395" t="s">
-        <v>644</v>
+        <v>594</v>
       </c>
     </row>
     <row r="396" spans="1:11">
@@ -16275,22 +16275,22 @@
         <v>565</v>
       </c>
       <c r="F396">
-        <v>55.10000000000001</v>
+        <v>51.30000000000001</v>
       </c>
       <c r="G396">
         <v>-25</v>
       </c>
       <c r="H396">
-        <v>8.866666666666667</v>
+        <v>10.86666666666667</v>
       </c>
       <c r="I396" t="s">
         <v>572</v>
       </c>
       <c r="J396">
-        <v>0.604422452</v>
+        <v>0.700977107</v>
       </c>
       <c r="K396" t="s">
-        <v>594</v>
+        <v>644</v>
       </c>
     </row>
     <row r="397" spans="1:11">
@@ -16395,7 +16395,7 @@
         <v>0.898196715</v>
       </c>
       <c r="K399" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="400" spans="1:11">
@@ -17007,25 +17007,25 @@
         <v>560</v>
       </c>
       <c r="E417" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="F417">
-        <v>39.90000000000146</v>
+        <v>50.20000000000073</v>
       </c>
       <c r="G417">
-        <v>-27</v>
+        <v>-30</v>
       </c>
       <c r="H417">
-        <v>10.55</v>
+        <v>8.883333333333333</v>
       </c>
       <c r="I417" t="s">
         <v>572</v>
       </c>
       <c r="J417">
-        <v>0.6724663670000001</v>
+        <v>1</v>
       </c>
       <c r="K417" t="s">
-        <v>624</v>
+        <v>668</v>
       </c>
     </row>
     <row r="418" spans="1:11">
@@ -17042,25 +17042,25 @@
         <v>560</v>
       </c>
       <c r="E418" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
       <c r="F418">
-        <v>50.20000000000073</v>
+        <v>39.90000000000146</v>
       </c>
       <c r="G418">
-        <v>-30</v>
+        <v>-27</v>
       </c>
       <c r="H418">
-        <v>8.883333333333333</v>
+        <v>10.55</v>
       </c>
       <c r="I418" t="s">
         <v>572</v>
       </c>
       <c r="J418">
-        <v>1</v>
+        <v>0.6724663670000001</v>
       </c>
       <c r="K418" t="s">
-        <v>668</v>
+        <v>624</v>
       </c>
     </row>
     <row r="419" spans="1:11">
@@ -17185,22 +17185,22 @@
         <v>565</v>
       </c>
       <c r="F422">
-        <v>41.7</v>
+        <v>43.6</v>
       </c>
       <c r="G422">
-        <v>-25</v>
+        <v>-20</v>
       </c>
       <c r="H422">
-        <v>7.733333333333333</v>
+        <v>10.9</v>
       </c>
       <c r="I422" t="s">
         <v>572</v>
       </c>
       <c r="J422">
-        <v>1</v>
+        <v>0.434668865</v>
       </c>
       <c r="K422" t="s">
-        <v>603</v>
+        <v>576</v>
       </c>
     </row>
     <row r="423" spans="1:11">
@@ -17252,25 +17252,25 @@
         <v>560</v>
       </c>
       <c r="E424" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F424">
-        <v>43.6</v>
+        <v>44.40000000000001</v>
       </c>
       <c r="G424">
-        <v>-20</v>
+        <v>-35</v>
       </c>
       <c r="H424">
-        <v>10.9</v>
+        <v>9.15</v>
       </c>
       <c r="I424" t="s">
         <v>572</v>
       </c>
       <c r="J424">
-        <v>0.434668865</v>
+        <v>1</v>
       </c>
       <c r="K424" t="s">
-        <v>576</v>
+        <v>607</v>
       </c>
     </row>
     <row r="425" spans="1:11">
@@ -17287,16 +17287,16 @@
         <v>560</v>
       </c>
       <c r="E425" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="F425">
-        <v>44.40000000000001</v>
+        <v>41.7</v>
       </c>
       <c r="G425">
-        <v>-35</v>
+        <v>-25</v>
       </c>
       <c r="H425">
-        <v>9.15</v>
+        <v>7.733333333333333</v>
       </c>
       <c r="I425" t="s">
         <v>572</v>
@@ -17305,7 +17305,7 @@
         <v>1</v>
       </c>
       <c r="K425" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
     </row>
     <row r="426" spans="1:11">
@@ -17707,25 +17707,25 @@
         <v>560</v>
       </c>
       <c r="E437" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="F437">
-        <v>57.69999999999709</v>
+        <v>63.20000000000073</v>
       </c>
       <c r="G437">
         <v>-30</v>
       </c>
       <c r="H437">
-        <v>9.316666666666666</v>
+        <v>10.25</v>
       </c>
       <c r="I437" t="s">
         <v>575</v>
       </c>
       <c r="J437">
-        <v>0.714428417</v>
+        <v>0.434668865</v>
       </c>
       <c r="K437" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
     </row>
     <row r="438" spans="1:11">
@@ -17742,25 +17742,25 @@
         <v>560</v>
       </c>
       <c r="E438" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="F438">
-        <v>63.20000000000073</v>
+        <v>57.69999999999709</v>
       </c>
       <c r="G438">
         <v>-30</v>
       </c>
       <c r="H438">
-        <v>10.25</v>
+        <v>9.316666666666666</v>
       </c>
       <c r="I438" t="s">
         <v>575</v>
       </c>
       <c r="J438">
-        <v>0.434668865</v>
+        <v>0.714428417</v>
       </c>
       <c r="K438" t="s">
-        <v>576</v>
+        <v>581</v>
       </c>
     </row>
     <row r="439" spans="1:11">
@@ -18250,7 +18250,7 @@
         <v>0.8440999890000001</v>
       </c>
       <c r="K452" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="453" spans="1:11">
@@ -18932,25 +18932,25 @@
         <v>560</v>
       </c>
       <c r="E472" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F472">
-        <v>64.30000000000291</v>
+        <v>52.5</v>
       </c>
       <c r="G472">
         <v>-40</v>
       </c>
       <c r="H472">
-        <v>7.35</v>
+        <v>8.216666666666667</v>
       </c>
       <c r="I472" t="s">
         <v>572</v>
       </c>
       <c r="J472">
-        <v>0.434668865</v>
+        <v>0.756093405</v>
       </c>
       <c r="K472" t="s">
-        <v>576</v>
+        <v>584</v>
       </c>
     </row>
     <row r="473" spans="1:11">
@@ -18967,25 +18967,25 @@
         <v>560</v>
       </c>
       <c r="E473" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F473">
         <v>52.5</v>
       </c>
       <c r="G473">
-        <v>-40</v>
+        <v>-35</v>
       </c>
       <c r="H473">
-        <v>8.216666666666667</v>
+        <v>9.333333333333334</v>
       </c>
       <c r="I473" t="s">
         <v>572</v>
       </c>
       <c r="J473">
-        <v>0.756093405</v>
+        <v>1</v>
       </c>
       <c r="K473" t="s">
-        <v>584</v>
+        <v>648</v>
       </c>
     </row>
     <row r="474" spans="1:11">
@@ -19002,25 +19002,25 @@
         <v>560</v>
       </c>
       <c r="E474" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="F474">
-        <v>52.5</v>
+        <v>64.30000000000291</v>
       </c>
       <c r="G474">
-        <v>-35</v>
+        <v>-40</v>
       </c>
       <c r="H474">
-        <v>9.333333333333334</v>
+        <v>7.35</v>
       </c>
       <c r="I474" t="s">
         <v>572</v>
       </c>
       <c r="J474">
-        <v>1</v>
+        <v>0.434668865</v>
       </c>
       <c r="K474" t="s">
-        <v>648</v>
+        <v>576</v>
       </c>
     </row>
     <row r="475" spans="1:11">
@@ -19075,13 +19075,13 @@
         <v>565</v>
       </c>
       <c r="F476">
-        <v>35.79999999999927</v>
+        <v>64.09999999999854</v>
       </c>
       <c r="G476">
-        <v>-31</v>
+        <v>-40</v>
       </c>
       <c r="H476">
-        <v>6</v>
+        <v>8.15</v>
       </c>
       <c r="I476" t="s">
         <v>572</v>
@@ -19090,7 +19090,7 @@
         <v>1</v>
       </c>
       <c r="K476" t="s">
-        <v>586</v>
+        <v>681</v>
       </c>
     </row>
     <row r="477" spans="1:11">
@@ -19110,13 +19110,13 @@
         <v>565</v>
       </c>
       <c r="F477">
-        <v>64.09999999999854</v>
+        <v>35.79999999999927</v>
       </c>
       <c r="G477">
-        <v>-40</v>
+        <v>-31</v>
       </c>
       <c r="H477">
-        <v>8.15</v>
+        <v>6</v>
       </c>
       <c r="I477" t="s">
         <v>572</v>
@@ -19125,7 +19125,7 @@
         <v>1</v>
       </c>
       <c r="K477" t="s">
-        <v>681</v>
+        <v>586</v>
       </c>
     </row>
     <row r="478" spans="1:11">
@@ -19177,25 +19177,25 @@
         <v>560</v>
       </c>
       <c r="E479" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="F479">
-        <v>55.60000000000218</v>
+        <v>48.20000000000073</v>
       </c>
       <c r="G479">
         <v>-30</v>
       </c>
       <c r="H479">
-        <v>9</v>
+        <v>6.933333333333334</v>
       </c>
       <c r="I479" t="s">
         <v>572</v>
       </c>
       <c r="J479">
-        <v>1</v>
+        <v>0.807432802</v>
       </c>
       <c r="K479" t="s">
-        <v>639</v>
+        <v>653</v>
       </c>
     </row>
     <row r="480" spans="1:11">
@@ -19215,22 +19215,22 @@
         <v>565</v>
       </c>
       <c r="F480">
-        <v>48.20000000000073</v>
+        <v>31.10000000000218</v>
       </c>
       <c r="G480">
-        <v>-30</v>
+        <v>-31</v>
       </c>
       <c r="H480">
-        <v>6.933333333333334</v>
+        <v>8.766666666666667</v>
       </c>
       <c r="I480" t="s">
         <v>572</v>
       </c>
       <c r="J480">
-        <v>0.807432802</v>
+        <v>1</v>
       </c>
       <c r="K480" t="s">
-        <v>653</v>
+        <v>626</v>
       </c>
     </row>
     <row r="481" spans="1:11">
@@ -19247,16 +19247,16 @@
         <v>560</v>
       </c>
       <c r="E481" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F481">
-        <v>31.10000000000218</v>
+        <v>55.60000000000218</v>
       </c>
       <c r="G481">
-        <v>-31</v>
+        <v>-30</v>
       </c>
       <c r="H481">
-        <v>8.766666666666667</v>
+        <v>9</v>
       </c>
       <c r="I481" t="s">
         <v>572</v>
@@ -19265,7 +19265,7 @@
         <v>1</v>
       </c>
       <c r="K481" t="s">
-        <v>626</v>
+        <v>639</v>
       </c>
     </row>
     <row r="482" spans="1:11">
@@ -19405,7 +19405,7 @@
         <v>0.8440999890000001</v>
       </c>
       <c r="K485" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="486" spans="1:11">
@@ -19772,16 +19772,16 @@
         <v>560</v>
       </c>
       <c r="E496" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="F496">
-        <v>64.10000000000218</v>
+        <v>105.6000000000022</v>
       </c>
       <c r="G496">
         <v>-40</v>
       </c>
       <c r="H496">
-        <v>8.233333333333333</v>
+        <v>14.1</v>
       </c>
       <c r="I496" t="s">
         <v>572</v>
@@ -19790,7 +19790,7 @@
         <v>1</v>
       </c>
       <c r="K496" t="s">
-        <v>675</v>
+        <v>627</v>
       </c>
     </row>
     <row r="497" spans="1:11">
@@ -19810,13 +19810,13 @@
         <v>568</v>
       </c>
       <c r="F497">
-        <v>59.29999999999927</v>
+        <v>68.09999999999854</v>
       </c>
       <c r="G497">
-        <v>-40</v>
+        <v>-20</v>
       </c>
       <c r="H497">
-        <v>7.65</v>
+        <v>9</v>
       </c>
       <c r="I497" t="s">
         <v>572</v>
@@ -19825,7 +19825,7 @@
         <v>1</v>
       </c>
       <c r="K497" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
     </row>
     <row r="498" spans="1:11">
@@ -19842,16 +19842,16 @@
         <v>560</v>
       </c>
       <c r="E498" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F498">
-        <v>58.60000000000218</v>
+        <v>51.20000000000073</v>
       </c>
       <c r="G498">
-        <v>-22</v>
+        <v>-30</v>
       </c>
       <c r="H498">
-        <v>11.78333333333333</v>
+        <v>10.58333333333333</v>
       </c>
       <c r="I498" t="s">
         <v>572</v>
@@ -19860,7 +19860,7 @@
         <v>1</v>
       </c>
       <c r="K498" t="s">
-        <v>616</v>
+        <v>675</v>
       </c>
     </row>
     <row r="499" spans="1:11">
@@ -19877,16 +19877,16 @@
         <v>560</v>
       </c>
       <c r="E499" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="F499">
-        <v>51.20000000000073</v>
+        <v>59.29999999999927</v>
       </c>
       <c r="G499">
-        <v>-30</v>
+        <v>-40</v>
       </c>
       <c r="H499">
-        <v>10.58333333333333</v>
+        <v>7.65</v>
       </c>
       <c r="I499" t="s">
         <v>572</v>
@@ -19912,16 +19912,16 @@
         <v>560</v>
       </c>
       <c r="E500" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="F500">
-        <v>47.70000000000073</v>
+        <v>58.60000000000218</v>
       </c>
       <c r="G500">
-        <v>-30</v>
+        <v>-22</v>
       </c>
       <c r="H500">
-        <v>8.716666666666667</v>
+        <v>11.78333333333333</v>
       </c>
       <c r="I500" t="s">
         <v>572</v>
@@ -19930,7 +19930,7 @@
         <v>1</v>
       </c>
       <c r="K500" t="s">
-        <v>675</v>
+        <v>616</v>
       </c>
     </row>
     <row r="501" spans="1:11">
@@ -19947,16 +19947,16 @@
         <v>560</v>
       </c>
       <c r="E501" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F501">
-        <v>59</v>
+        <v>47.70000000000073</v>
       </c>
       <c r="G501">
-        <v>-36</v>
+        <v>-30</v>
       </c>
       <c r="H501">
-        <v>7.333333333333333</v>
+        <v>8.716666666666667</v>
       </c>
       <c r="I501" t="s">
         <v>572</v>
@@ -19965,7 +19965,7 @@
         <v>1</v>
       </c>
       <c r="K501" t="s">
-        <v>578</v>
+        <v>675</v>
       </c>
     </row>
     <row r="502" spans="1:11">
@@ -19985,13 +19985,13 @@
         <v>565</v>
       </c>
       <c r="F502">
-        <v>105.6000000000022</v>
+        <v>59</v>
       </c>
       <c r="G502">
-        <v>-40</v>
+        <v>-36</v>
       </c>
       <c r="H502">
-        <v>14.1</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="I502" t="s">
         <v>572</v>
@@ -20000,7 +20000,7 @@
         <v>1</v>
       </c>
       <c r="K502" t="s">
-        <v>627</v>
+        <v>578</v>
       </c>
     </row>
     <row r="503" spans="1:11">
@@ -20017,16 +20017,16 @@
         <v>560</v>
       </c>
       <c r="E503" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="F503">
-        <v>68.09999999999854</v>
+        <v>64.10000000000218</v>
       </c>
       <c r="G503">
-        <v>-20</v>
+        <v>-40</v>
       </c>
       <c r="H503">
-        <v>9</v>
+        <v>8.233333333333333</v>
       </c>
       <c r="I503" t="s">
         <v>572</v>
@@ -20035,7 +20035,7 @@
         <v>1</v>
       </c>
       <c r="K503" t="s">
-        <v>669</v>
+        <v>675</v>
       </c>
     </row>
     <row r="504" spans="1:11">
@@ -20052,25 +20052,25 @@
         <v>560</v>
       </c>
       <c r="E504" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F504">
         <v>43.70000000000073</v>
       </c>
       <c r="G504">
-        <v>-25</v>
+        <v>-26</v>
       </c>
       <c r="H504">
-        <v>11.33333333333333</v>
+        <v>13.1</v>
       </c>
       <c r="I504" t="s">
         <v>572</v>
       </c>
       <c r="J504">
-        <v>0.714428417</v>
+        <v>0.8682376890000001</v>
       </c>
       <c r="K504" t="s">
-        <v>581</v>
+        <v>619</v>
       </c>
     </row>
     <row r="505" spans="1:11">
@@ -20087,25 +20087,25 @@
         <v>560</v>
       </c>
       <c r="E505" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F505">
         <v>43.70000000000073</v>
       </c>
       <c r="G505">
-        <v>-26</v>
+        <v>-25</v>
       </c>
       <c r="H505">
-        <v>13.1</v>
+        <v>11.33333333333333</v>
       </c>
       <c r="I505" t="s">
         <v>572</v>
       </c>
       <c r="J505">
-        <v>0.8682376890000001</v>
+        <v>0.714428417</v>
       </c>
       <c r="K505" t="s">
-        <v>619</v>
+        <v>581</v>
       </c>
     </row>
     <row r="506" spans="1:11">
@@ -20300,22 +20300,22 @@
         <v>563</v>
       </c>
       <c r="F511">
-        <v>53.40000000000146</v>
+        <v>65.70000000000073</v>
       </c>
       <c r="G511">
-        <v>-40</v>
+        <v>-31</v>
       </c>
       <c r="H511">
-        <v>9.083333333333334</v>
+        <v>10.2</v>
       </c>
       <c r="I511" t="s">
         <v>572</v>
       </c>
       <c r="J511">
-        <v>1</v>
+        <v>0.9144092620000001</v>
       </c>
       <c r="K511" t="s">
-        <v>684</v>
+        <v>599</v>
       </c>
     </row>
     <row r="512" spans="1:11">
@@ -20335,22 +20335,22 @@
         <v>563</v>
       </c>
       <c r="F512">
-        <v>65.70000000000073</v>
+        <v>53.40000000000146</v>
       </c>
       <c r="G512">
-        <v>-31</v>
+        <v>-40</v>
       </c>
       <c r="H512">
-        <v>10.2</v>
+        <v>9.083333333333334</v>
       </c>
       <c r="I512" t="s">
         <v>572</v>
       </c>
       <c r="J512">
-        <v>0.9144092620000001</v>
+        <v>1</v>
       </c>
       <c r="K512" t="s">
-        <v>599</v>
+        <v>684</v>
       </c>
     </row>
     <row r="513" spans="1:11">
@@ -20370,22 +20370,22 @@
         <v>565</v>
       </c>
       <c r="F513">
-        <v>46.89999999999782</v>
+        <v>52.60000000000218</v>
       </c>
       <c r="G513">
-        <v>-40</v>
+        <v>-38</v>
       </c>
       <c r="H513">
-        <v>7.95</v>
+        <v>9.9</v>
       </c>
       <c r="I513" t="s">
         <v>572</v>
       </c>
       <c r="J513">
-        <v>0.874431515</v>
+        <v>1</v>
       </c>
       <c r="K513" t="s">
-        <v>617</v>
+        <v>578</v>
       </c>
     </row>
     <row r="514" spans="1:11">
@@ -20402,16 +20402,16 @@
         <v>560</v>
       </c>
       <c r="E514" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="F514">
-        <v>44.5</v>
+        <v>62.09999999999855</v>
       </c>
       <c r="G514">
         <v>-40</v>
       </c>
       <c r="H514">
-        <v>7.883333333333334</v>
+        <v>7.966666666666667</v>
       </c>
       <c r="I514" t="s">
         <v>572</v>
@@ -20437,25 +20437,25 @@
         <v>560</v>
       </c>
       <c r="E515" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F515">
-        <v>52.60000000000218</v>
+        <v>44.5</v>
       </c>
       <c r="G515">
-        <v>-38</v>
+        <v>-40</v>
       </c>
       <c r="H515">
-        <v>9.9</v>
+        <v>7.883333333333334</v>
       </c>
       <c r="I515" t="s">
         <v>572</v>
       </c>
       <c r="J515">
-        <v>1</v>
+        <v>0.291080192</v>
       </c>
       <c r="K515" t="s">
-        <v>578</v>
+        <v>590</v>
       </c>
     </row>
     <row r="516" spans="1:11">
@@ -20472,25 +20472,25 @@
         <v>560</v>
       </c>
       <c r="E516" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="F516">
-        <v>44.70000000000073</v>
+        <v>46.89999999999782</v>
       </c>
       <c r="G516">
-        <v>-35</v>
+        <v>-40</v>
       </c>
       <c r="H516">
-        <v>9.300000000000001</v>
+        <v>7.95</v>
       </c>
       <c r="I516" t="s">
         <v>572</v>
       </c>
       <c r="J516">
-        <v>1</v>
+        <v>0.874431515</v>
       </c>
       <c r="K516" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="517" spans="1:11">
@@ -20507,25 +20507,25 @@
         <v>560</v>
       </c>
       <c r="E517" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="F517">
-        <v>62.09999999999855</v>
+        <v>44.70000000000073</v>
       </c>
       <c r="G517">
-        <v>-40</v>
+        <v>-35</v>
       </c>
       <c r="H517">
-        <v>7.966666666666667</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="I517" t="s">
         <v>572</v>
       </c>
       <c r="J517">
-        <v>0.291080192</v>
+        <v>1</v>
       </c>
       <c r="K517" t="s">
-        <v>590</v>
+        <v>616</v>
       </c>
     </row>
     <row r="518" spans="1:11">
@@ -20650,22 +20650,22 @@
         <v>565</v>
       </c>
       <c r="F521">
-        <v>59.29999999999927</v>
+        <v>66.20000000000073</v>
       </c>
       <c r="G521">
-        <v>-40</v>
+        <v>-30</v>
       </c>
       <c r="H521">
-        <v>6.816666666666666</v>
+        <v>15.16666666666667</v>
       </c>
       <c r="I521" t="s">
         <v>572</v>
       </c>
       <c r="J521">
-        <v>1</v>
+        <v>0.434668865</v>
       </c>
       <c r="K521" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="522" spans="1:11">
@@ -20685,22 +20685,22 @@
         <v>565</v>
       </c>
       <c r="F522">
-        <v>66.20000000000073</v>
+        <v>59.29999999999927</v>
       </c>
       <c r="G522">
-        <v>-30</v>
+        <v>-40</v>
       </c>
       <c r="H522">
-        <v>15.16666666666667</v>
+        <v>6.816666666666666</v>
       </c>
       <c r="I522" t="s">
         <v>572</v>
       </c>
       <c r="J522">
-        <v>0.434668865</v>
+        <v>1</v>
       </c>
       <c r="K522" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
     </row>
     <row r="523" spans="1:11">
@@ -20895,22 +20895,22 @@
         <v>565</v>
       </c>
       <c r="F528">
-        <v>57.59999999999855</v>
+        <v>52.20000000000073</v>
       </c>
       <c r="G528">
-        <v>-40</v>
+        <v>-42</v>
       </c>
       <c r="H528">
-        <v>7.516666666666667</v>
+        <v>10.55</v>
       </c>
       <c r="I528" t="s">
         <v>572</v>
       </c>
       <c r="J528">
-        <v>0.700977107</v>
+        <v>1</v>
       </c>
       <c r="K528" t="s">
-        <v>644</v>
+        <v>596</v>
       </c>
     </row>
     <row r="529" spans="1:11">
@@ -21000,22 +21000,22 @@
         <v>565</v>
       </c>
       <c r="F531">
-        <v>52.20000000000073</v>
+        <v>57.59999999999855</v>
       </c>
       <c r="G531">
-        <v>-42</v>
+        <v>-40</v>
       </c>
       <c r="H531">
-        <v>10.55</v>
+        <v>7.516666666666667</v>
       </c>
       <c r="I531" t="s">
         <v>572</v>
       </c>
       <c r="J531">
-        <v>1</v>
+        <v>0.700977107</v>
       </c>
       <c r="K531" t="s">
-        <v>596</v>
+        <v>644</v>
       </c>
     </row>
     <row r="532" spans="1:11">
@@ -21035,22 +21035,22 @@
         <v>565</v>
       </c>
       <c r="F532">
-        <v>63.10000000000218</v>
+        <v>63.79999999999927</v>
       </c>
       <c r="G532">
-        <v>-30</v>
+        <v>-40</v>
       </c>
       <c r="H532">
-        <v>7.45</v>
+        <v>6.8</v>
       </c>
       <c r="I532" t="s">
         <v>572</v>
       </c>
       <c r="J532">
-        <v>0.8440999890000001</v>
+        <v>1</v>
       </c>
       <c r="K532" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
     </row>
     <row r="533" spans="1:11">
@@ -21070,22 +21070,22 @@
         <v>565</v>
       </c>
       <c r="F533">
-        <v>55.69999999999709</v>
+        <v>63.10000000000218</v>
       </c>
       <c r="G533">
-        <v>-40</v>
+        <v>-30</v>
       </c>
       <c r="H533">
-        <v>7.65</v>
+        <v>7.45</v>
       </c>
       <c r="I533" t="s">
         <v>572</v>
       </c>
       <c r="J533">
-        <v>1</v>
+        <v>0.8440999890000001</v>
       </c>
       <c r="K533" t="s">
-        <v>627</v>
+        <v>633</v>
       </c>
     </row>
     <row r="534" spans="1:11">
@@ -21140,22 +21140,22 @@
         <v>565</v>
       </c>
       <c r="F535">
-        <v>40.10000000000218</v>
+        <v>48.5</v>
       </c>
       <c r="G535">
         <v>-30</v>
       </c>
       <c r="H535">
-        <v>7.383333333333334</v>
+        <v>7.883333333333334</v>
       </c>
       <c r="I535" t="s">
         <v>572</v>
       </c>
       <c r="J535">
-        <v>1</v>
+        <v>0.8440999890000001</v>
       </c>
       <c r="K535" t="s">
-        <v>686</v>
+        <v>633</v>
       </c>
     </row>
     <row r="536" spans="1:11">
@@ -21175,13 +21175,13 @@
         <v>565</v>
       </c>
       <c r="F536">
-        <v>63.79999999999927</v>
+        <v>55.69999999999709</v>
       </c>
       <c r="G536">
         <v>-40</v>
       </c>
       <c r="H536">
-        <v>6.8</v>
+        <v>7.65</v>
       </c>
       <c r="I536" t="s">
         <v>572</v>
@@ -21210,22 +21210,22 @@
         <v>565</v>
       </c>
       <c r="F537">
-        <v>48.5</v>
+        <v>40.10000000000218</v>
       </c>
       <c r="G537">
         <v>-30</v>
       </c>
       <c r="H537">
-        <v>7.883333333333334</v>
+        <v>7.383333333333334</v>
       </c>
       <c r="I537" t="s">
         <v>572</v>
       </c>
       <c r="J537">
-        <v>0.8440999890000001</v>
+        <v>1</v>
       </c>
       <c r="K537" t="s">
-        <v>632</v>
+        <v>686</v>
       </c>
     </row>
     <row r="538" spans="1:11">
@@ -21347,25 +21347,25 @@
         <v>560</v>
       </c>
       <c r="E541" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F541">
-        <v>54.89999999999782</v>
+        <v>63.79999999999927</v>
       </c>
       <c r="G541">
-        <v>-20</v>
+        <v>-40</v>
       </c>
       <c r="H541">
-        <v>10.41666666666667</v>
+        <v>6.85</v>
       </c>
       <c r="I541" t="s">
         <v>572</v>
       </c>
       <c r="J541">
-        <v>1</v>
+        <v>0.700977107</v>
       </c>
       <c r="K541" t="s">
-        <v>582</v>
+        <v>644</v>
       </c>
     </row>
     <row r="542" spans="1:11">
@@ -21385,22 +21385,22 @@
         <v>565</v>
       </c>
       <c r="F542">
-        <v>63.79999999999927</v>
+        <v>60.5</v>
       </c>
       <c r="G542">
-        <v>-40</v>
+        <v>-30</v>
       </c>
       <c r="H542">
-        <v>6.85</v>
+        <v>7.833333333333333</v>
       </c>
       <c r="I542" t="s">
         <v>572</v>
       </c>
       <c r="J542">
-        <v>0.700977107</v>
+        <v>1</v>
       </c>
       <c r="K542" t="s">
-        <v>644</v>
+        <v>582</v>
       </c>
     </row>
     <row r="543" spans="1:11">
@@ -21417,16 +21417,16 @@
         <v>560</v>
       </c>
       <c r="E543" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="F543">
-        <v>60.5</v>
+        <v>54.89999999999782</v>
       </c>
       <c r="G543">
-        <v>-30</v>
+        <v>-20</v>
       </c>
       <c r="H543">
-        <v>7.833333333333333</v>
+        <v>10.41666666666667</v>
       </c>
       <c r="I543" t="s">
         <v>572</v>
@@ -21522,25 +21522,25 @@
         <v>560</v>
       </c>
       <c r="E546" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F546">
-        <v>66.79999999999927</v>
+        <v>61.89999999999782</v>
       </c>
       <c r="G546">
         <v>-40</v>
       </c>
       <c r="H546">
-        <v>6.416666666666667</v>
+        <v>9.416666666666666</v>
       </c>
       <c r="I546" t="s">
         <v>572</v>
       </c>
       <c r="J546">
-        <v>0.714428417</v>
+        <v>1</v>
       </c>
       <c r="K546" t="s">
-        <v>581</v>
+        <v>627</v>
       </c>
     </row>
     <row r="547" spans="1:11">
@@ -21557,25 +21557,25 @@
         <v>560</v>
       </c>
       <c r="E547" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="F547">
-        <v>61.89999999999782</v>
+        <v>66.79999999999927</v>
       </c>
       <c r="G547">
         <v>-40</v>
       </c>
       <c r="H547">
-        <v>9.416666666666666</v>
+        <v>6.416666666666667</v>
       </c>
       <c r="I547" t="s">
         <v>572</v>
       </c>
       <c r="J547">
-        <v>1</v>
+        <v>0.714428417</v>
       </c>
       <c r="K547" t="s">
-        <v>627</v>
+        <v>581</v>
       </c>
     </row>
     <row r="548" spans="1:11">
@@ -21592,25 +21592,25 @@
         <v>560</v>
       </c>
       <c r="E548" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="F548">
-        <v>47</v>
+        <v>67.09999999999854</v>
       </c>
       <c r="G548">
-        <v>-35</v>
+        <v>-40</v>
       </c>
       <c r="H548">
-        <v>9.5</v>
+        <v>9.883333333333333</v>
       </c>
       <c r="I548" t="s">
         <v>572</v>
       </c>
       <c r="J548">
-        <v>0.860418943</v>
+        <v>1</v>
       </c>
       <c r="K548" t="s">
-        <v>635</v>
+        <v>663</v>
       </c>
     </row>
     <row r="549" spans="1:11">
@@ -21629,20 +21629,23 @@
       <c r="E549" t="s">
         <v>564</v>
       </c>
+      <c r="F549">
+        <v>47</v>
+      </c>
       <c r="G549">
-        <v>-37</v>
+        <v>-35</v>
       </c>
       <c r="H549">
-        <v>12.56666666666667</v>
+        <v>9.5</v>
       </c>
       <c r="I549" t="s">
         <v>572</v>
       </c>
       <c r="J549">
-        <v>0.86644284</v>
+        <v>0.860418943</v>
       </c>
       <c r="K549" t="s">
-        <v>678</v>
+        <v>635</v>
       </c>
     </row>
     <row r="550" spans="1:11">
@@ -21659,25 +21662,22 @@
         <v>560</v>
       </c>
       <c r="E550" t="s">
-        <v>568</v>
-      </c>
-      <c r="F550">
-        <v>67.09999999999854</v>
+        <v>564</v>
       </c>
       <c r="G550">
-        <v>-40</v>
+        <v>-37</v>
       </c>
       <c r="H550">
-        <v>9.883333333333333</v>
+        <v>12.56666666666667</v>
       </c>
       <c r="I550" t="s">
         <v>572</v>
       </c>
       <c r="J550">
-        <v>1</v>
+        <v>0.86644284</v>
       </c>
       <c r="K550" t="s">
-        <v>663</v>
+        <v>678</v>
       </c>
     </row>
     <row r="551" spans="1:11">

</xml_diff>